<commit_message>
read test cases from excels and create final json files
</commit_message>
<xml_diff>
--- a/src/test/resources/test_descriptions/Thefreedictionary_TestCases.xlsx
+++ b/src/test/resources/test_descriptions/Thefreedictionary_TestCases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\project\UITest2Code\src\test\resources\test_descriptions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7831BC0E-99E5-4DAF-B36D-6A9197D22AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BFEAD3-1D0F-4B4F-AD87-72C1770C91D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{90D935EE-D077-954D-8ED4-802E55CBA7B8}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="15600" xr2:uid="{90D935EE-D077-954D-8ED4-802E55CBA7B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="133">
   <si>
     <t>Homepage-Setings - Language</t>
   </si>
@@ -480,12 +480,30 @@
   <si>
     <t>SK_17</t>
   </si>
+  <si>
+    <t>Test Case ID</t>
+  </si>
+  <si>
+    <t>Test Name</t>
+  </si>
+  <si>
+    <t>Test Description</t>
+  </si>
+  <si>
+    <t>Preconditions</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Expected Results</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -528,6 +546,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Trebuchet MS"/>
       <family val="2"/>
     </font>
@@ -582,7 +615,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -843,11 +876,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -967,25 +1015,16 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1008,6 +1047,21 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1322,10 +1376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9040D4-FA61-D147-9C70-571311E7A7B4}">
-  <dimension ref="A1:F175"/>
+  <dimension ref="A1:F176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C142" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E177" sqref="E177"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1337,198 +1391,210 @@
     <col min="6" max="6" width="92.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="58" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="59" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="59" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="59" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" s="59" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="2" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="35"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="35"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="1"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="E3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="35"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="46"/>
       <c r="D4" s="1"/>
       <c r="E4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="35"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="44"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="46"/>
       <c r="D5" s="1"/>
       <c r="E5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="35"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="44"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="46"/>
       <c r="D6" s="1"/>
       <c r="E6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="35"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="44"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="35"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="44"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="1"/>
       <c r="E8" s="2"/>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="35"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="44"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="1"/>
       <c r="E9" s="2"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="37"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
+    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="35"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="46"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" ht="19.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="45" t="s">
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="37"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" ht="19.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-    </row>
-    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="46" t="s">
+      <c r="B12" s="55"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+    </row>
+    <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B13" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C13" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="49" t="s">
+      <c r="D13" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="35"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="E13" s="1"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A14" s="35"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="50"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="47"/>
       <c r="E14" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A15" s="35"/>
-      <c r="B15" s="43"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="50"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="47"/>
       <c r="E15" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A16" s="35"/>
-      <c r="B16" s="43"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="1" t="s">
-        <v>13</v>
+      <c r="B16" s="45"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A17" s="35"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="50"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="47"/>
       <c r="E17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A18" s="35"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="50"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="47"/>
       <c r="E18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="35"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="1"/>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
@@ -1547,39 +1613,37 @@
       <c r="E21" s="1"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="37"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="35" t="s">
+    <row r="22" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="36"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="37"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="B23" s="43" t="s">
+      <c r="B24" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="44" t="s">
+      <c r="C24" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="50" t="s">
+      <c r="D24" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="36"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="4"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A25" s="36"/>
@@ -1587,27 +1651,27 @@
       <c r="C25" s="36"/>
       <c r="D25" s="36"/>
       <c r="E25" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="82.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A26" s="36"/>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
       <c r="D26" s="36"/>
       <c r="E26" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="82.5" x14ac:dyDescent="0.2">
       <c r="A27" s="36"/>
       <c r="B27" s="36"/>
       <c r="C27" s="36"/>
       <c r="D27" s="36"/>
       <c r="E27" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F27" s="4"/>
     </row>
@@ -1617,7 +1681,7 @@
       <c r="C28" s="36"/>
       <c r="D28" s="36"/>
       <c r="E28" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F28" s="4"/>
     </row>
@@ -1626,7 +1690,9 @@
       <c r="B29" s="36"/>
       <c r="C29" s="36"/>
       <c r="D29" s="36"/>
-      <c r="E29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
@@ -1645,273 +1711,271 @@
       <c r="E31" s="1"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="37"/>
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="35" t="s">
+    <row r="32" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A32" s="36"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="37"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="B33" s="43" t="s">
+      <c r="B34" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="44" t="s">
+      <c r="C34" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="50" t="s">
+      <c r="D34" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E33" s="8"/>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A34" s="35"/>
-      <c r="B34" s="43"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="50"/>
-      <c r="E34" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="E34" s="8"/>
       <c r="F34" s="2"/>
     </row>
     <row r="35" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A35" s="35"/>
-      <c r="B35" s="43"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="50"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="47"/>
       <c r="E35" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F35" s="2"/>
     </row>
     <row r="36" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A36" s="35"/>
-      <c r="B36" s="43"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="8" t="s">
+      <c r="B36" s="45"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="35"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="1:6" ht="49.5" x14ac:dyDescent="0.2">
-      <c r="A37" s="35"/>
-      <c r="B37" s="43"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="50"/>
-      <c r="E37" s="8" t="s">
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:6" ht="49.5" x14ac:dyDescent="0.2">
+      <c r="A38" s="35"/>
+      <c r="B38" s="45"/>
+      <c r="C38" s="46"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F38" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A38" s="35"/>
-      <c r="B38" s="43"/>
-      <c r="C38" s="44"/>
-      <c r="D38" s="50"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="2"/>
-    </row>
     <row r="39" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="4"/>
-    </row>
-    <row r="40" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="37"/>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="7"/>
-    </row>
-    <row r="41" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="35" t="s">
+      <c r="A39" s="35"/>
+      <c r="B39" s="45"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A40" s="36"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="37"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="B41" s="43" t="s">
+      <c r="B42" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="44" t="s">
+      <c r="C42" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="D41" s="50" t="s">
+      <c r="D42" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E41" s="8"/>
-      <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="35"/>
-      <c r="B42" s="43"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="50"/>
-      <c r="E42" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="E42" s="8"/>
       <c r="F42" s="2"/>
     </row>
     <row r="43" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A43" s="35"/>
-      <c r="B43" s="43"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="50"/>
+      <c r="B43" s="45"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="47"/>
       <c r="E43" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F43" s="2"/>
     </row>
     <row r="44" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A44" s="35"/>
-      <c r="B44" s="43"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="50"/>
-      <c r="E44" s="8" t="s">
+      <c r="B44" s="45"/>
+      <c r="C44" s="46"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A45" s="35"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="1:6" ht="49.5" x14ac:dyDescent="0.2">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F45" s="4"/>
-    </row>
-    <row r="46" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:6" ht="49.5" x14ac:dyDescent="0.2">
       <c r="A46" s="36"/>
       <c r="B46" s="36"/>
       <c r="C46" s="36"/>
       <c r="D46" s="36"/>
-      <c r="E46" s="1" t="s">
-        <v>30</v>
+      <c r="E46" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="1:6" ht="33" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A47" s="36"/>
       <c r="B47" s="36"/>
       <c r="C47" s="36"/>
       <c r="D47" s="36"/>
       <c r="E47" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F47" s="4"/>
     </row>
-    <row r="48" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" ht="33" x14ac:dyDescent="0.2">
       <c r="A48" s="36"/>
       <c r="B48" s="36"/>
       <c r="C48" s="36"/>
       <c r="D48" s="36"/>
-      <c r="E48" s="1"/>
+      <c r="E48" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="F48" s="4"/>
     </row>
-    <row r="49" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="37"/>
-      <c r="B49" s="37"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="37"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="7"/>
-    </row>
-    <row r="50" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="35" t="s">
+    <row r="49" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A49" s="36"/>
+      <c r="B49" s="36"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="37"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="37"/>
+      <c r="D50" s="37"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="7"/>
+    </row>
+    <row r="51" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="B50" s="43" t="s">
+      <c r="B51" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="C50" s="44" t="s">
+      <c r="C51" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="D50" s="50" t="s">
+      <c r="D51" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E50" s="8"/>
-      <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A51" s="35"/>
-      <c r="B51" s="43"/>
-      <c r="C51" s="44"/>
-      <c r="D51" s="50"/>
-      <c r="E51" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="E51" s="8"/>
       <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A52" s="35"/>
-      <c r="B52" s="43"/>
-      <c r="C52" s="44"/>
-      <c r="D52" s="50"/>
+      <c r="B52" s="45"/>
+      <c r="C52" s="46"/>
+      <c r="D52" s="47"/>
       <c r="E52" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A53" s="35"/>
-      <c r="B53" s="43"/>
-      <c r="C53" s="44"/>
-      <c r="D53" s="50"/>
-      <c r="E53" s="8" t="s">
+      <c r="B53" s="45"/>
+      <c r="C53" s="46"/>
+      <c r="D53" s="47"/>
+      <c r="E53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53" s="2"/>
+    </row>
+    <row r="54" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A54" s="35"/>
+      <c r="B54" s="45"/>
+      <c r="C54" s="46"/>
+      <c r="D54" s="47"/>
+      <c r="E54" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F53" s="2"/>
-    </row>
-    <row r="54" spans="1:6" ht="49.5" x14ac:dyDescent="0.2">
-      <c r="A54" s="35"/>
-      <c r="B54" s="43"/>
-      <c r="C54" s="44"/>
-      <c r="D54" s="50"/>
-      <c r="E54" s="8" t="s">
+      <c r="F54" s="2"/>
+    </row>
+    <row r="55" spans="1:6" ht="49.5" x14ac:dyDescent="0.2">
+      <c r="A55" s="35"/>
+      <c r="B55" s="45"/>
+      <c r="C55" s="46"/>
+      <c r="D55" s="47"/>
+      <c r="E55" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F54" s="2"/>
-    </row>
-    <row r="55" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A55" s="35"/>
-      <c r="B55" s="43"/>
-      <c r="C55" s="44"/>
-      <c r="D55" s="50"/>
-      <c r="E55" s="1" t="s">
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A56" s="35"/>
+      <c r="B56" s="45"/>
+      <c r="C56" s="46"/>
+      <c r="D56" s="47"/>
+      <c r="E56" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F55" s="2"/>
-    </row>
-    <row r="56" spans="1:6" ht="33" x14ac:dyDescent="0.2">
-      <c r="A56" s="35"/>
-      <c r="B56" s="43"/>
-      <c r="C56" s="44"/>
-      <c r="D56" s="50"/>
-      <c r="E56" s="1" t="s">
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="1:6" ht="33" x14ac:dyDescent="0.2">
+      <c r="A57" s="35"/>
+      <c r="B57" s="45"/>
+      <c r="C57" s="46"/>
+      <c r="D57" s="47"/>
+      <c r="E57" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F56" s="2"/>
-    </row>
-    <row r="57" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A57" s="36"/>
-      <c r="B57" s="36"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F57" s="4"/>
+      <c r="F57" s="2"/>
     </row>
     <row r="58" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A58" s="36"/>
@@ -1919,113 +1983,113 @@
       <c r="C58" s="36"/>
       <c r="D58" s="36"/>
       <c r="E58" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F58" s="4" t="s">
-        <v>36</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="F58" s="4"/>
     </row>
     <row r="59" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A59" s="36"/>
       <c r="B59" s="36"/>
       <c r="C59" s="36"/>
       <c r="D59" s="36"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="4"/>
-    </row>
-    <row r="60" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="37"/>
-      <c r="B60" s="37"/>
-      <c r="C60" s="37"/>
-      <c r="D60" s="37"/>
-      <c r="E60" s="6"/>
-      <c r="F60" s="7"/>
-    </row>
-    <row r="61" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="35" t="s">
+      <c r="E59" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A60" s="36"/>
+      <c r="B60" s="36"/>
+      <c r="C60" s="36"/>
+      <c r="D60" s="36"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="4"/>
+    </row>
+    <row r="61" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="37"/>
+      <c r="B61" s="37"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="37"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="7"/>
+    </row>
+    <row r="62" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="B61" s="43" t="s">
+      <c r="B62" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C61" s="44" t="s">
+      <c r="C62" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="D61" s="50" t="s">
+      <c r="D62" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E61" s="8"/>
-      <c r="F61" s="2"/>
-    </row>
-    <row r="62" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A62" s="35"/>
-      <c r="B62" s="43"/>
-      <c r="C62" s="44"/>
-      <c r="D62" s="50"/>
-      <c r="E62" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="E62" s="8"/>
       <c r="F62" s="2"/>
     </row>
     <row r="63" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A63" s="35"/>
-      <c r="B63" s="43"/>
-      <c r="C63" s="44"/>
-      <c r="D63" s="50"/>
+      <c r="B63" s="45"/>
+      <c r="C63" s="46"/>
+      <c r="D63" s="47"/>
       <c r="E63" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F63" s="2"/>
     </row>
     <row r="64" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A64" s="35"/>
-      <c r="B64" s="43"/>
-      <c r="C64" s="44"/>
-      <c r="D64" s="50"/>
-      <c r="E64" s="8" t="s">
+      <c r="B64" s="45"/>
+      <c r="C64" s="46"/>
+      <c r="D64" s="47"/>
+      <c r="E64" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A65" s="35"/>
+      <c r="B65" s="45"/>
+      <c r="C65" s="46"/>
+      <c r="D65" s="47"/>
+      <c r="E65" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F64" s="2"/>
-    </row>
-    <row r="65" spans="1:6" ht="49.5" x14ac:dyDescent="0.2">
-      <c r="A65" s="35"/>
-      <c r="B65" s="43"/>
-      <c r="C65" s="44"/>
-      <c r="D65" s="50"/>
-      <c r="E65" s="8" t="s">
+      <c r="F65" s="2"/>
+    </row>
+    <row r="66" spans="1:6" ht="49.5" x14ac:dyDescent="0.2">
+      <c r="A66" s="35"/>
+      <c r="B66" s="45"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="47"/>
+      <c r="E66" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F65" s="2"/>
-    </row>
-    <row r="66" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A66" s="35"/>
-      <c r="B66" s="43"/>
-      <c r="C66" s="44"/>
-      <c r="D66" s="50"/>
-      <c r="E66" s="1" t="s">
+      <c r="F66" s="2"/>
+    </row>
+    <row r="67" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A67" s="35"/>
+      <c r="B67" s="45"/>
+      <c r="C67" s="46"/>
+      <c r="D67" s="47"/>
+      <c r="E67" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F66" s="2"/>
-    </row>
-    <row r="67" spans="1:6" ht="33" x14ac:dyDescent="0.2">
-      <c r="A67" s="35"/>
-      <c r="B67" s="43"/>
-      <c r="C67" s="44"/>
-      <c r="D67" s="50"/>
-      <c r="E67" s="1" t="s">
+      <c r="F67" s="2"/>
+    </row>
+    <row r="68" spans="1:6" ht="33" x14ac:dyDescent="0.2">
+      <c r="A68" s="35"/>
+      <c r="B68" s="45"/>
+      <c r="C68" s="46"/>
+      <c r="D68" s="47"/>
+      <c r="E68" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F67" s="2"/>
-    </row>
-    <row r="68" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A68" s="36"/>
-      <c r="B68" s="36"/>
-      <c r="C68" s="36"/>
-      <c r="D68" s="36"/>
-      <c r="E68" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F68" s="4"/>
+      <c r="F68" s="2"/>
     </row>
     <row r="69" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A69" s="36"/>
@@ -2033,19 +2097,21 @@
       <c r="C69" s="36"/>
       <c r="D69" s="36"/>
       <c r="E69" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>41</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="F69" s="4"/>
     </row>
     <row r="70" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A70" s="36"/>
       <c r="B70" s="36"/>
       <c r="C70" s="36"/>
       <c r="D70" s="36"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="4"/>
+      <c r="E70" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="71" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A71" s="36"/>
@@ -2063,106 +2129,106 @@
       <c r="E72" s="1"/>
       <c r="F72" s="4"/>
     </row>
-    <row r="73" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="37"/>
-      <c r="B73" s="37"/>
-      <c r="C73" s="37"/>
-      <c r="D73" s="37"/>
-      <c r="E73" s="6"/>
-      <c r="F73" s="7"/>
-    </row>
-    <row r="74" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="35" t="s">
+    <row r="73" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A73" s="36"/>
+      <c r="B73" s="36"/>
+      <c r="C73" s="36"/>
+      <c r="D73" s="36"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="4"/>
+    </row>
+    <row r="74" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="37"/>
+      <c r="B74" s="37"/>
+      <c r="C74" s="37"/>
+      <c r="D74" s="37"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="7"/>
+    </row>
+    <row r="75" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="B74" s="43" t="s">
+      <c r="B75" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="C74" s="44" t="s">
+      <c r="C75" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="D74" s="50" t="s">
+      <c r="D75" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E74" s="8"/>
-      <c r="F74" s="2"/>
-    </row>
-    <row r="75" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A75" s="35"/>
-      <c r="B75" s="43"/>
-      <c r="C75" s="44"/>
-      <c r="D75" s="50"/>
-      <c r="E75" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="E75" s="8"/>
       <c r="F75" s="2"/>
     </row>
     <row r="76" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A76" s="35"/>
-      <c r="B76" s="43"/>
-      <c r="C76" s="44"/>
-      <c r="D76" s="50"/>
+      <c r="B76" s="45"/>
+      <c r="C76" s="46"/>
+      <c r="D76" s="47"/>
       <c r="E76" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F76" s="2"/>
     </row>
     <row r="77" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A77" s="35"/>
-      <c r="B77" s="43"/>
-      <c r="C77" s="44"/>
-      <c r="D77" s="50"/>
-      <c r="E77" s="8" t="s">
-        <v>44</v>
+      <c r="B77" s="45"/>
+      <c r="C77" s="46"/>
+      <c r="D77" s="47"/>
+      <c r="E77" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="F77" s="2"/>
     </row>
     <row r="78" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A78" s="35"/>
-      <c r="B78" s="43"/>
-      <c r="C78" s="44"/>
-      <c r="D78" s="50"/>
+      <c r="B78" s="45"/>
+      <c r="C78" s="46"/>
+      <c r="D78" s="47"/>
       <c r="E78" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F78" s="2"/>
     </row>
     <row r="79" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A79" s="35"/>
-      <c r="B79" s="43"/>
-      <c r="C79" s="44"/>
-      <c r="D79" s="50"/>
+      <c r="B79" s="45"/>
+      <c r="C79" s="46"/>
+      <c r="D79" s="47"/>
       <c r="E79" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F79" s="2"/>
     </row>
     <row r="80" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A80" s="35"/>
-      <c r="B80" s="43"/>
-      <c r="C80" s="44"/>
-      <c r="D80" s="50"/>
+      <c r="B80" s="45"/>
+      <c r="C80" s="46"/>
+      <c r="D80" s="47"/>
       <c r="E80" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F80" s="2"/>
+    </row>
+    <row r="81" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A81" s="35"/>
+      <c r="B81" s="45"/>
+      <c r="C81" s="46"/>
+      <c r="D81" s="47"/>
+      <c r="E81" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F80" s="2"/>
-    </row>
-    <row r="81" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A81" s="36"/>
-      <c r="B81" s="36"/>
-      <c r="C81" s="36"/>
-      <c r="D81" s="36"/>
-      <c r="E81" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F81" s="4"/>
+      <c r="F81" s="2"/>
     </row>
     <row r="82" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A82" s="36"/>
       <c r="B82" s="36"/>
       <c r="C82" s="36"/>
       <c r="D82" s="36"/>
-      <c r="E82" s="1"/>
+      <c r="E82" s="9" t="s">
+        <v>48</v>
+      </c>
       <c r="F82" s="4"/>
     </row>
     <row r="83" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
@@ -2173,39 +2239,37 @@
       <c r="E83" s="1"/>
       <c r="F83" s="4"/>
     </row>
-    <row r="84" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="37"/>
-      <c r="B84" s="37"/>
-      <c r="C84" s="37"/>
-      <c r="D84" s="37"/>
-      <c r="E84" s="6"/>
-      <c r="F84" s="7"/>
-    </row>
-    <row r="85" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="35" t="s">
+    <row r="84" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A84" s="36"/>
+      <c r="B84" s="36"/>
+      <c r="C84" s="36"/>
+      <c r="D84" s="36"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="4"/>
+    </row>
+    <row r="85" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="37"/>
+      <c r="B85" s="37"/>
+      <c r="C85" s="37"/>
+      <c r="D85" s="37"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="7"/>
+    </row>
+    <row r="86" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="B85" s="43" t="s">
+      <c r="B86" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="C85" s="44" t="s">
+      <c r="C86" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="D85" s="50" t="s">
+      <c r="D86" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E85" s="8"/>
-      <c r="F85" s="2"/>
-    </row>
-    <row r="86" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A86" s="36"/>
-      <c r="B86" s="36"/>
-      <c r="C86" s="36"/>
-      <c r="D86" s="36"/>
-      <c r="E86" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F86" s="4"/>
+      <c r="E86" s="8"/>
+      <c r="F86" s="2"/>
     </row>
     <row r="87" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A87" s="36"/>
@@ -2213,7 +2277,7 @@
       <c r="C87" s="36"/>
       <c r="D87" s="36"/>
       <c r="E87" s="1" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="F87" s="4"/>
     </row>
@@ -2223,7 +2287,7 @@
       <c r="C88" s="36"/>
       <c r="D88" s="36"/>
       <c r="E88" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F88" s="4"/>
     </row>
@@ -2233,7 +2297,7 @@
       <c r="C89" s="36"/>
       <c r="D89" s="36"/>
       <c r="E89" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F89" s="4"/>
     </row>
@@ -2242,162 +2306,162 @@
       <c r="B90" s="36"/>
       <c r="C90" s="36"/>
       <c r="D90" s="36"/>
-      <c r="E90" s="1"/>
+      <c r="E90" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="F90" s="4"/>
     </row>
-    <row r="91" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="37"/>
+    <row r="91" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A91" s="36"/>
       <c r="B91" s="36"/>
-      <c r="C91" s="37"/>
-      <c r="D91" s="37"/>
-      <c r="E91" s="6"/>
-      <c r="F91" s="7"/>
-    </row>
-    <row r="92" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="51" t="s">
+      <c r="C91" s="36"/>
+      <c r="D91" s="36"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="4"/>
+    </row>
+    <row r="92" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="37"/>
+      <c r="B92" s="36"/>
+      <c r="C92" s="37"/>
+      <c r="D92" s="37"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="7"/>
+    </row>
+    <row r="93" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="B92" s="54" t="s">
+      <c r="B93" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="C92" s="41" t="s">
+      <c r="C93" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="D92" s="50" t="s">
+      <c r="D93" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E92" s="8"/>
-      <c r="F92" s="2"/>
-    </row>
-    <row r="93" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A93" s="52"/>
-      <c r="B93" s="55"/>
-      <c r="C93" s="41"/>
-      <c r="D93" s="50"/>
-      <c r="E93" s="8" t="s">
+      <c r="E93" s="8"/>
+      <c r="F93" s="2"/>
+    </row>
+    <row r="94" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A94" s="49"/>
+      <c r="B94" s="52"/>
+      <c r="C94" s="41"/>
+      <c r="D94" s="47"/>
+      <c r="E94" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F93" s="2"/>
-    </row>
-    <row r="94" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A94" s="52"/>
-      <c r="B94" s="55"/>
-      <c r="C94" s="41"/>
-      <c r="D94" s="50"/>
-      <c r="E94" s="8" t="s">
+      <c r="F94" s="2"/>
+    </row>
+    <row r="95" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A95" s="49"/>
+      <c r="B95" s="52"/>
+      <c r="C95" s="41"/>
+      <c r="D95" s="47"/>
+      <c r="E95" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F94" s="2"/>
-    </row>
-    <row r="95" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A95" s="52"/>
-      <c r="B95" s="55"/>
-      <c r="C95" s="41"/>
-      <c r="D95" s="50"/>
-      <c r="E95" s="8" t="s">
+      <c r="F95" s="2"/>
+    </row>
+    <row r="96" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A96" s="49"/>
+      <c r="B96" s="52"/>
+      <c r="C96" s="41"/>
+      <c r="D96" s="47"/>
+      <c r="E96" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F95" s="2"/>
-    </row>
-    <row r="96" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A96" s="52"/>
-      <c r="B96" s="55"/>
-      <c r="C96" s="41"/>
-      <c r="D96" s="50"/>
-      <c r="E96" s="8" t="s">
+      <c r="F96" s="2"/>
+    </row>
+    <row r="97" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A97" s="49"/>
+      <c r="B97" s="52"/>
+      <c r="C97" s="41"/>
+      <c r="D97" s="47"/>
+      <c r="E97" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="F96" s="2"/>
-    </row>
-    <row r="97" spans="1:6" ht="82.5" x14ac:dyDescent="0.2">
-      <c r="A97" s="52"/>
-      <c r="B97" s="55"/>
-      <c r="C97" s="41"/>
-      <c r="D97" s="50"/>
-      <c r="E97" s="8" t="s">
+      <c r="F97" s="2"/>
+    </row>
+    <row r="98" spans="1:6" ht="82.5" x14ac:dyDescent="0.2">
+      <c r="A98" s="49"/>
+      <c r="B98" s="52"/>
+      <c r="C98" s="41"/>
+      <c r="D98" s="47"/>
+      <c r="E98" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="F97" s="2"/>
-    </row>
-    <row r="98" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A98" s="52"/>
-      <c r="B98" s="55"/>
-      <c r="C98" s="41"/>
-      <c r="D98" s="50"/>
-      <c r="E98" s="8" t="s">
+      <c r="F98" s="2"/>
+    </row>
+    <row r="99" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A99" s="49"/>
+      <c r="B99" s="52"/>
+      <c r="C99" s="41"/>
+      <c r="D99" s="47"/>
+      <c r="E99" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F98" s="2"/>
-    </row>
-    <row r="99" spans="1:6" ht="49.5" x14ac:dyDescent="0.2">
-      <c r="A99" s="35"/>
-      <c r="B99" s="56"/>
-      <c r="C99" s="44"/>
-      <c r="D99" s="50"/>
-      <c r="E99" s="8" t="s">
+      <c r="F99" s="2"/>
+    </row>
+    <row r="100" spans="1:6" ht="49.5" x14ac:dyDescent="0.2">
+      <c r="A100" s="35"/>
+      <c r="B100" s="53"/>
+      <c r="C100" s="46"/>
+      <c r="D100" s="47"/>
+      <c r="E100" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="F99" s="2"/>
-    </row>
-    <row r="100" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A100" s="35"/>
-      <c r="B100" s="36"/>
-      <c r="C100" s="36"/>
-      <c r="D100" s="36"/>
-      <c r="E100" s="1"/>
-      <c r="F100" s="4"/>
-    </row>
-    <row r="101" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="53"/>
-      <c r="B101" s="57"/>
-      <c r="C101" s="37"/>
-      <c r="D101" s="37"/>
-      <c r="E101" s="6"/>
-      <c r="F101" s="7"/>
-    </row>
-    <row r="102" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="35" t="s">
+      <c r="F100" s="2"/>
+    </row>
+    <row r="101" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A101" s="35"/>
+      <c r="B101" s="36"/>
+      <c r="C101" s="36"/>
+      <c r="D101" s="36"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="4"/>
+    </row>
+    <row r="102" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="50"/>
+      <c r="B102" s="54"/>
+      <c r="C102" s="37"/>
+      <c r="D102" s="37"/>
+      <c r="E102" s="6"/>
+      <c r="F102" s="7"/>
+    </row>
+    <row r="103" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="B102" s="43" t="s">
+      <c r="B103" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="C102" s="44" t="s">
+      <c r="C103" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="D102" s="50" t="s">
+      <c r="D103" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E102" s="8"/>
-      <c r="F102" s="2"/>
-    </row>
-    <row r="103" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A103" s="36"/>
-      <c r="B103" s="36"/>
-      <c r="C103" s="36"/>
-      <c r="D103" s="36"/>
-      <c r="E103" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F103" s="4"/>
-    </row>
-    <row r="104" spans="1:6" ht="33" x14ac:dyDescent="0.2">
+      <c r="E103" s="8"/>
+      <c r="F103" s="2"/>
+    </row>
+    <row r="104" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A104" s="36"/>
       <c r="B104" s="36"/>
       <c r="C104" s="36"/>
       <c r="D104" s="36"/>
-      <c r="E104" s="1" t="s">
-        <v>64</v>
+      <c r="E104" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="F104" s="4"/>
     </row>
-    <row r="105" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" ht="33" x14ac:dyDescent="0.2">
       <c r="A105" s="36"/>
       <c r="B105" s="36"/>
       <c r="C105" s="36"/>
       <c r="D105" s="36"/>
       <c r="E105" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F105" s="4"/>
     </row>
@@ -2407,7 +2471,7 @@
       <c r="C106" s="36"/>
       <c r="D106" s="36"/>
       <c r="E106" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F106" s="4"/>
     </row>
@@ -2416,7 +2480,9 @@
       <c r="B107" s="36"/>
       <c r="C107" s="36"/>
       <c r="D107" s="36"/>
-      <c r="E107" s="1"/>
+      <c r="E107" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="F107" s="4"/>
     </row>
     <row r="108" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
@@ -2451,75 +2517,75 @@
       <c r="E111" s="1"/>
       <c r="F111" s="4"/>
     </row>
-    <row r="112" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="37"/>
-      <c r="B112" s="37"/>
-      <c r="C112" s="37"/>
-      <c r="D112" s="37"/>
+    <row r="112" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A112" s="36"/>
+      <c r="B112" s="36"/>
+      <c r="C112" s="36"/>
+      <c r="D112" s="36"/>
       <c r="E112" s="1"/>
       <c r="F112" s="4"/>
     </row>
-    <row r="113" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="35" t="s">
+    <row r="113" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="37"/>
+      <c r="B113" s="37"/>
+      <c r="C113" s="37"/>
+      <c r="D113" s="37"/>
+      <c r="E113" s="1"/>
+      <c r="F113" s="4"/>
+    </row>
+    <row r="114" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="B113" s="38" t="s">
+      <c r="B114" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="C113" s="41" t="s">
+      <c r="C114" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="D113" s="42" t="s">
+      <c r="D114" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E113" s="10"/>
-      <c r="F113" s="11"/>
-    </row>
-    <row r="114" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A114" s="35"/>
-      <c r="B114" s="38"/>
-      <c r="C114" s="41"/>
-      <c r="D114" s="42"/>
-      <c r="E114" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F114" s="12"/>
+      <c r="E114" s="10"/>
+      <c r="F114" s="11"/>
     </row>
     <row r="115" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A115" s="35"/>
       <c r="B115" s="38"/>
       <c r="C115" s="41"/>
       <c r="D115" s="42"/>
-      <c r="E115" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="F115" s="14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E115" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F115" s="12"/>
+    </row>
+    <row r="116" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A116" s="35"/>
       <c r="B116" s="38"/>
       <c r="C116" s="41"/>
       <c r="D116" s="42"/>
-      <c r="E116" s="15"/>
-      <c r="F116" s="12"/>
+      <c r="E116" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F116" s="14" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A117" s="36"/>
-      <c r="B117" s="39"/>
-      <c r="C117" s="39"/>
-      <c r="D117" s="39"/>
-      <c r="E117" s="16"/>
-      <c r="F117" s="17"/>
-    </row>
-    <row r="118" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A117" s="35"/>
+      <c r="B117" s="38"/>
+      <c r="C117" s="41"/>
+      <c r="D117" s="42"/>
+      <c r="E117" s="15"/>
+      <c r="F117" s="12"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="36"/>
       <c r="B118" s="39"/>
       <c r="C118" s="39"/>
       <c r="D118" s="39"/>
-      <c r="E118" s="8"/>
-      <c r="F118" s="12"/>
+      <c r="E118" s="16"/>
+      <c r="F118" s="17"/>
     </row>
     <row r="119" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A119" s="36"/>
@@ -2527,7 +2593,7 @@
       <c r="C119" s="39"/>
       <c r="D119" s="39"/>
       <c r="E119" s="8"/>
-      <c r="F119" s="17"/>
+      <c r="F119" s="12"/>
     </row>
     <row r="120" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A120" s="36"/>
@@ -2535,40 +2601,38 @@
       <c r="C120" s="39"/>
       <c r="D120" s="39"/>
       <c r="E120" s="8"/>
-      <c r="F120" s="12"/>
-    </row>
-    <row r="121" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="37"/>
-      <c r="B121" s="40"/>
-      <c r="C121" s="40"/>
-      <c r="D121" s="40"/>
-      <c r="E121" s="18"/>
-      <c r="F121" s="19"/>
-    </row>
-    <row r="122" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="35" t="s">
+      <c r="F120" s="17"/>
+    </row>
+    <row r="121" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A121" s="36"/>
+      <c r="B121" s="39"/>
+      <c r="C121" s="39"/>
+      <c r="D121" s="39"/>
+      <c r="E121" s="8"/>
+      <c r="F121" s="12"/>
+    </row>
+    <row r="122" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="37"/>
+      <c r="B122" s="40"/>
+      <c r="C122" s="40"/>
+      <c r="D122" s="40"/>
+      <c r="E122" s="18"/>
+      <c r="F122" s="19"/>
+    </row>
+    <row r="123" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="B122" s="38" t="s">
+      <c r="B123" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="C122" s="41" t="s">
+      <c r="C123" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="D122" s="42" t="s">
+      <c r="D123" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E122" s="20"/>
-      <c r="F122" s="21"/>
-    </row>
-    <row r="123" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A123" s="35"/>
-      <c r="B123" s="38"/>
-      <c r="C123" s="41"/>
-      <c r="D123" s="42"/>
-      <c r="E123" s="8" t="s">
-        <v>12</v>
-      </c>
+      <c r="E123" s="20"/>
       <c r="F123" s="21"/>
     </row>
     <row r="124" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
@@ -2576,30 +2640,30 @@
       <c r="B124" s="38"/>
       <c r="C124" s="41"/>
       <c r="D124" s="42"/>
-      <c r="E124" s="22" t="s">
+      <c r="E124" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F124" s="21"/>
+    </row>
+    <row r="125" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A125" s="35"/>
+      <c r="B125" s="38"/>
+      <c r="C125" s="41"/>
+      <c r="D125" s="42"/>
+      <c r="E125" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="F124" s="21"/>
-    </row>
-    <row r="125" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A125" s="36"/>
-      <c r="B125" s="39"/>
-      <c r="C125" s="39"/>
-      <c r="D125" s="39"/>
-      <c r="E125" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="F125" s="24"/>
+      <c r="F125" s="21"/>
     </row>
     <row r="126" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A126" s="36"/>
       <c r="B126" s="39"/>
       <c r="C126" s="39"/>
       <c r="D126" s="39"/>
-      <c r="E126" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="F126" s="26"/>
+      <c r="E126" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="F126" s="24"/>
     </row>
     <row r="127" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A127" s="36"/>
@@ -2607,11 +2671,9 @@
       <c r="C127" s="39"/>
       <c r="D127" s="39"/>
       <c r="E127" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="F127" s="27" t="s">
-        <v>77</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F127" s="26"/>
     </row>
     <row r="128" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A128" s="36"/>
@@ -2619,63 +2681,65 @@
       <c r="C128" s="39"/>
       <c r="D128" s="39"/>
       <c r="E128" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="F128" s="27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A129" s="36"/>
+      <c r="B129" s="39"/>
+      <c r="C129" s="39"/>
+      <c r="D129" s="39"/>
+      <c r="E129" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="F128" s="24"/>
-    </row>
-    <row r="129" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="37"/>
-      <c r="B129" s="40"/>
-      <c r="C129" s="40"/>
-      <c r="D129" s="40"/>
-      <c r="E129" s="18"/>
-      <c r="F129" s="19"/>
-    </row>
-    <row r="130" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="35" t="s">
+      <c r="F129" s="24"/>
+    </row>
+    <row r="130" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="37"/>
+      <c r="B130" s="40"/>
+      <c r="C130" s="40"/>
+      <c r="D130" s="40"/>
+      <c r="E130" s="18"/>
+      <c r="F130" s="19"/>
+    </row>
+    <row r="131" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="B130" s="38" t="s">
+      <c r="B131" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="C130" s="41" t="s">
+      <c r="C131" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="D130" s="42" t="s">
+      <c r="D131" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E130" s="28"/>
-      <c r="F130" s="26"/>
-    </row>
-    <row r="131" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A131" s="36"/>
-      <c r="B131" s="39"/>
-      <c r="C131" s="39"/>
-      <c r="D131" s="39"/>
-      <c r="E131" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F131" s="24"/>
-    </row>
-    <row r="132" spans="1:6" ht="33" x14ac:dyDescent="0.2">
+      <c r="E131" s="28"/>
+      <c r="F131" s="26"/>
+    </row>
+    <row r="132" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A132" s="36"/>
       <c r="B132" s="39"/>
       <c r="C132" s="39"/>
       <c r="D132" s="39"/>
-      <c r="E132" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F132" s="26"/>
-    </row>
-    <row r="133" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="E132" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F132" s="24"/>
+    </row>
+    <row r="133" spans="1:6" ht="33" x14ac:dyDescent="0.2">
       <c r="A133" s="36"/>
       <c r="B133" s="39"/>
       <c r="C133" s="39"/>
       <c r="D133" s="39"/>
       <c r="E133" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F133" s="24"/>
+        <v>81</v>
+      </c>
+      <c r="F133" s="26"/>
     </row>
     <row r="134" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A134" s="36"/>
@@ -2683,17 +2747,19 @@
       <c r="C134" s="39"/>
       <c r="D134" s="39"/>
       <c r="E134" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F134" s="29"/>
+        <v>65</v>
+      </c>
+      <c r="F134" s="24"/>
     </row>
     <row r="135" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A135" s="36"/>
       <c r="B135" s="39"/>
       <c r="C135" s="39"/>
       <c r="D135" s="39"/>
-      <c r="E135" s="25"/>
-      <c r="F135" s="26"/>
+      <c r="E135" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F135" s="29"/>
     </row>
     <row r="136" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A136" s="36"/>
@@ -2701,59 +2767,57 @@
       <c r="C136" s="39"/>
       <c r="D136" s="39"/>
       <c r="E136" s="25"/>
-      <c r="F136" s="24"/>
-    </row>
-    <row r="137" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="37"/>
-      <c r="B137" s="40"/>
-      <c r="C137" s="40"/>
-      <c r="D137" s="40"/>
-      <c r="E137" s="18"/>
-      <c r="F137" s="19"/>
-    </row>
-    <row r="138" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="35" t="s">
+      <c r="F136" s="26"/>
+    </row>
+    <row r="137" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A137" s="36"/>
+      <c r="B137" s="39"/>
+      <c r="C137" s="39"/>
+      <c r="D137" s="39"/>
+      <c r="E137" s="25"/>
+      <c r="F137" s="24"/>
+    </row>
+    <row r="138" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="37"/>
+      <c r="B138" s="40"/>
+      <c r="C138" s="40"/>
+      <c r="D138" s="40"/>
+      <c r="E138" s="18"/>
+      <c r="F138" s="19"/>
+    </row>
+    <row r="139" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="B138" s="38" t="s">
+      <c r="B139" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="C138" s="48" t="s">
+      <c r="C139" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="D138" s="49" t="s">
+      <c r="D139" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="E138" s="28"/>
-      <c r="F138" s="26"/>
-    </row>
-    <row r="139" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A139" s="36"/>
-      <c r="B139" s="39"/>
-      <c r="C139" s="36"/>
-      <c r="D139" s="36"/>
-      <c r="E139" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F139" s="24"/>
-    </row>
-    <row r="140" spans="1:6" ht="33" x14ac:dyDescent="0.2">
+      <c r="E139" s="28"/>
+      <c r="F139" s="26"/>
+    </row>
+    <row r="140" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A140" s="36"/>
       <c r="B140" s="39"/>
       <c r="C140" s="36"/>
       <c r="D140" s="36"/>
-      <c r="E140" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F140" s="26"/>
-    </row>
-    <row r="141" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="E140" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F140" s="24"/>
+    </row>
+    <row r="141" spans="1:6" ht="33" x14ac:dyDescent="0.2">
       <c r="A141" s="36"/>
       <c r="B141" s="39"/>
       <c r="C141" s="36"/>
       <c r="D141" s="36"/>
       <c r="E141" s="1" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="F141" s="26"/>
     </row>
@@ -2763,7 +2827,7 @@
       <c r="C142" s="36"/>
       <c r="D142" s="36"/>
       <c r="E142" s="1" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="F142" s="26"/>
     </row>
@@ -2772,8 +2836,8 @@
       <c r="B143" s="39"/>
       <c r="C143" s="36"/>
       <c r="D143" s="36"/>
-      <c r="E143" s="25" t="s">
-        <v>85</v>
+      <c r="E143" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="F143" s="26"/>
     </row>
@@ -2783,81 +2847,81 @@
       <c r="C144" s="36"/>
       <c r="D144" s="36"/>
       <c r="E144" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="F144" s="24"/>
+        <v>85</v>
+      </c>
+      <c r="F144" s="26"/>
     </row>
     <row r="145" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A145" s="36"/>
       <c r="B145" s="39"/>
       <c r="C145" s="36"/>
       <c r="D145" s="36"/>
-      <c r="E145" s="25"/>
+      <c r="E145" s="25" t="s">
+        <v>86</v>
+      </c>
       <c r="F145" s="24"/>
     </row>
-    <row r="146" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="37"/>
-      <c r="B146" s="40"/>
-      <c r="C146" s="37"/>
-      <c r="D146" s="37"/>
-      <c r="E146" s="18"/>
-      <c r="F146" s="30"/>
-    </row>
-    <row r="147" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="35" t="s">
+    <row r="146" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A146" s="36"/>
+      <c r="B146" s="39"/>
+      <c r="C146" s="36"/>
+      <c r="D146" s="36"/>
+      <c r="E146" s="25"/>
+      <c r="F146" s="24"/>
+    </row>
+    <row r="147" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="37"/>
+      <c r="B147" s="40"/>
+      <c r="C147" s="37"/>
+      <c r="D147" s="37"/>
+      <c r="E147" s="18"/>
+      <c r="F147" s="30"/>
+    </row>
+    <row r="148" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="B147" s="43" t="s">
+      <c r="B148" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="C147" s="41" t="s">
+      <c r="C148" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="D147" s="42" t="s">
+      <c r="D148" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E147" s="28"/>
-      <c r="F147" s="21"/>
-    </row>
-    <row r="148" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A148" s="35"/>
-      <c r="B148" s="43"/>
-      <c r="C148" s="41"/>
-      <c r="D148" s="42"/>
-      <c r="E148" s="8" t="s">
-        <v>12</v>
-      </c>
+      <c r="E148" s="28"/>
       <c r="F148" s="21"/>
     </row>
     <row r="149" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A149" s="35"/>
-      <c r="B149" s="43"/>
+      <c r="B149" s="45"/>
       <c r="C149" s="41"/>
       <c r="D149" s="42"/>
-      <c r="E149" s="31" t="s">
+      <c r="E149" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F149" s="21"/>
+    </row>
+    <row r="150" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A150" s="35"/>
+      <c r="B150" s="45"/>
+      <c r="C150" s="41"/>
+      <c r="D150" s="42"/>
+      <c r="E150" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="F149" s="21"/>
-    </row>
-    <row r="150" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A150" s="36"/>
-      <c r="B150" s="36"/>
-      <c r="C150" s="39"/>
-      <c r="D150" s="39"/>
-      <c r="E150" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="F150" s="24"/>
+      <c r="F150" s="21"/>
     </row>
     <row r="151" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A151" s="36"/>
       <c r="B151" s="36"/>
       <c r="C151" s="39"/>
       <c r="D151" s="39"/>
-      <c r="E151" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="F151" s="26"/>
+      <c r="E151" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="F151" s="24"/>
     </row>
     <row r="152" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A152" s="36"/>
@@ -2865,73 +2929,75 @@
       <c r="C152" s="39"/>
       <c r="D152" s="39"/>
       <c r="E152" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="F152" s="26"/>
+    </row>
+    <row r="153" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A153" s="36"/>
+      <c r="B153" s="36"/>
+      <c r="C153" s="39"/>
+      <c r="D153" s="39"/>
+      <c r="E153" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="F152" s="24"/>
-    </row>
-    <row r="153" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="37"/>
-      <c r="B153" s="37"/>
-      <c r="C153" s="40"/>
-      <c r="D153" s="40"/>
-      <c r="E153" s="32"/>
-      <c r="F153" s="33"/>
-    </row>
-    <row r="154" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="35" t="s">
+      <c r="F153" s="24"/>
+    </row>
+    <row r="154" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="37"/>
+      <c r="B154" s="37"/>
+      <c r="C154" s="40"/>
+      <c r="D154" s="40"/>
+      <c r="E154" s="32"/>
+      <c r="F154" s="33"/>
+    </row>
+    <row r="155" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="B154" s="38" t="s">
+      <c r="B155" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="C154" s="41" t="s">
+      <c r="C155" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="D154" s="42" t="s">
+      <c r="D155" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E154" s="28"/>
-      <c r="F154" s="26"/>
-    </row>
-    <row r="155" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A155" s="36"/>
-      <c r="B155" s="39"/>
-      <c r="C155" s="39"/>
-      <c r="D155" s="39"/>
-      <c r="E155" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F155" s="24"/>
+      <c r="E155" s="28"/>
+      <c r="F155" s="26"/>
     </row>
     <row r="156" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A156" s="36"/>
       <c r="B156" s="39"/>
       <c r="C156" s="39"/>
       <c r="D156" s="39"/>
-      <c r="E156" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="F156" s="26"/>
-    </row>
-    <row r="157" spans="1:6" ht="49.5" x14ac:dyDescent="0.2">
+      <c r="E156" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F156" s="24"/>
+    </row>
+    <row r="157" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A157" s="36"/>
       <c r="B157" s="39"/>
       <c r="C157" s="39"/>
       <c r="D157" s="39"/>
-      <c r="E157" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="F157" s="27" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="E157" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="F157" s="26"/>
+    </row>
+    <row r="158" spans="1:6" ht="49.5" x14ac:dyDescent="0.2">
       <c r="A158" s="36"/>
       <c r="B158" s="39"/>
       <c r="C158" s="39"/>
       <c r="D158" s="39"/>
-      <c r="E158" s="25"/>
-      <c r="F158" s="24"/>
+      <c r="E158" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="F158" s="27" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="159" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A159" s="36"/>
@@ -2941,69 +3007,67 @@
       <c r="E159" s="25"/>
       <c r="F159" s="24"/>
     </row>
-    <row r="160" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="37"/>
-      <c r="B160" s="40"/>
-      <c r="C160" s="40"/>
-      <c r="D160" s="40"/>
-      <c r="E160" s="18"/>
-      <c r="F160" s="19"/>
-    </row>
-    <row r="161" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A161" s="35" t="s">
+    <row r="160" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A160" s="36"/>
+      <c r="B160" s="39"/>
+      <c r="C160" s="39"/>
+      <c r="D160" s="39"/>
+      <c r="E160" s="25"/>
+      <c r="F160" s="24"/>
+    </row>
+    <row r="161" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="37"/>
+      <c r="B161" s="40"/>
+      <c r="C161" s="40"/>
+      <c r="D161" s="40"/>
+      <c r="E161" s="18"/>
+      <c r="F161" s="19"/>
+    </row>
+    <row r="162" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="B161" s="38" t="s">
+      <c r="B162" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="C161" s="41" t="s">
+      <c r="C162" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="D161" s="42" t="s">
+      <c r="D162" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E161" s="28"/>
-      <c r="F161" s="26"/>
-    </row>
-    <row r="162" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A162" s="36"/>
-      <c r="B162" s="39"/>
-      <c r="C162" s="39"/>
-      <c r="D162" s="39"/>
-      <c r="E162" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F162" s="24"/>
+      <c r="E162" s="28"/>
+      <c r="F162" s="26"/>
     </row>
     <row r="163" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A163" s="36"/>
       <c r="B163" s="39"/>
       <c r="C163" s="39"/>
       <c r="D163" s="39"/>
-      <c r="E163" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="F163" s="26"/>
+      <c r="E163" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F163" s="24"/>
     </row>
     <row r="164" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A164" s="36"/>
       <c r="B164" s="39"/>
       <c r="C164" s="39"/>
       <c r="D164" s="39"/>
-      <c r="E164" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="F164" s="27"/>
+      <c r="E164" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="F164" s="26"/>
     </row>
     <row r="165" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A165" s="36"/>
       <c r="B165" s="39"/>
       <c r="C165" s="39"/>
       <c r="D165" s="39"/>
-      <c r="E165" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="F165" s="24"/>
+      <c r="E165" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="F165" s="27"/>
     </row>
     <row r="166" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A166" s="36"/>
@@ -3011,71 +3075,73 @@
       <c r="C166" s="39"/>
       <c r="D166" s="39"/>
       <c r="E166" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="F166" s="24"/>
+    </row>
+    <row r="167" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A167" s="36"/>
+      <c r="B167" s="39"/>
+      <c r="C167" s="39"/>
+      <c r="D167" s="39"/>
+      <c r="E167" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="F166" s="24"/>
-    </row>
-    <row r="167" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="37"/>
-      <c r="B167" s="40"/>
-      <c r="C167" s="40"/>
-      <c r="D167" s="40"/>
-      <c r="E167" s="18"/>
-      <c r="F167" s="19"/>
-    </row>
-    <row r="168" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A168" s="35" t="s">
+      <c r="F167" s="24"/>
+    </row>
+    <row r="168" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="37"/>
+      <c r="B168" s="40"/>
+      <c r="C168" s="40"/>
+      <c r="D168" s="40"/>
+      <c r="E168" s="18"/>
+      <c r="F168" s="19"/>
+    </row>
+    <row r="169" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A169" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="B168" s="38" t="s">
+      <c r="B169" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="C168" s="41" t="s">
+      <c r="C169" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="D168" s="42" t="s">
+      <c r="D169" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E168" s="28"/>
-      <c r="F168" s="26"/>
-    </row>
-    <row r="169" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A169" s="36"/>
-      <c r="B169" s="39"/>
-      <c r="C169" s="39"/>
-      <c r="D169" s="39"/>
-      <c r="E169" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="F169" s="24"/>
+      <c r="E169" s="28"/>
+      <c r="F169" s="26"/>
     </row>
     <row r="170" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A170" s="36"/>
       <c r="B170" s="39"/>
       <c r="C170" s="39"/>
       <c r="D170" s="39"/>
-      <c r="E170" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="F170" s="26" t="s">
-        <v>107</v>
-      </c>
+      <c r="E170" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F170" s="24"/>
     </row>
     <row r="171" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A171" s="36"/>
       <c r="B171" s="39"/>
       <c r="C171" s="39"/>
       <c r="D171" s="39"/>
-      <c r="E171" s="34"/>
-      <c r="F171" s="27"/>
+      <c r="E171" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F171" s="26" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="172" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A172" s="36"/>
       <c r="B172" s="39"/>
       <c r="C172" s="39"/>
       <c r="D172" s="39"/>
-      <c r="E172" s="25"/>
-      <c r="F172" s="24"/>
+      <c r="E172" s="34"/>
+      <c r="F172" s="27"/>
     </row>
     <row r="173" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A173" s="36"/>
@@ -3085,97 +3151,106 @@
       <c r="E173" s="25"/>
       <c r="F173" s="24"/>
     </row>
-    <row r="174" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="37"/>
-      <c r="B174" s="40"/>
-      <c r="C174" s="40"/>
-      <c r="D174" s="40"/>
-      <c r="E174" s="18"/>
-      <c r="F174" s="19"/>
-    </row>
-    <row r="175" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="174" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A174" s="36"/>
+      <c r="B174" s="39"/>
+      <c r="C174" s="39"/>
+      <c r="D174" s="39"/>
+      <c r="E174" s="25"/>
+      <c r="F174" s="24"/>
+    </row>
+    <row r="175" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="37"/>
+      <c r="B175" s="40"/>
+      <c r="C175" s="40"/>
+      <c r="D175" s="40"/>
+      <c r="E175" s="18"/>
+      <c r="F175" s="19"/>
+    </row>
+    <row r="176" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="A154:A160"/>
-    <mergeCell ref="B154:B160"/>
-    <mergeCell ref="C154:C160"/>
-    <mergeCell ref="D154:D160"/>
-    <mergeCell ref="A138:A146"/>
-    <mergeCell ref="B138:B146"/>
-    <mergeCell ref="C138:C146"/>
-    <mergeCell ref="D138:D146"/>
-    <mergeCell ref="A147:A153"/>
-    <mergeCell ref="B147:B153"/>
-    <mergeCell ref="C147:C153"/>
-    <mergeCell ref="D147:D153"/>
-    <mergeCell ref="A122:A129"/>
-    <mergeCell ref="B122:B129"/>
-    <mergeCell ref="C122:C129"/>
-    <mergeCell ref="D122:D129"/>
-    <mergeCell ref="A130:A137"/>
-    <mergeCell ref="B130:B137"/>
-    <mergeCell ref="C130:C137"/>
-    <mergeCell ref="D130:D137"/>
-    <mergeCell ref="A102:A112"/>
-    <mergeCell ref="B102:B112"/>
-    <mergeCell ref="C102:C112"/>
-    <mergeCell ref="D102:D112"/>
-    <mergeCell ref="A113:A121"/>
-    <mergeCell ref="B113:B121"/>
-    <mergeCell ref="C113:C121"/>
-    <mergeCell ref="D113:D121"/>
-    <mergeCell ref="A85:A91"/>
-    <mergeCell ref="B85:B91"/>
-    <mergeCell ref="C85:C91"/>
-    <mergeCell ref="D85:D91"/>
-    <mergeCell ref="A92:A101"/>
-    <mergeCell ref="B92:B98"/>
-    <mergeCell ref="C92:C101"/>
-    <mergeCell ref="D92:D101"/>
-    <mergeCell ref="B99:B101"/>
-    <mergeCell ref="A61:A73"/>
-    <mergeCell ref="B61:B73"/>
-    <mergeCell ref="C61:C73"/>
-    <mergeCell ref="D61:D73"/>
-    <mergeCell ref="A74:A84"/>
-    <mergeCell ref="B74:B84"/>
-    <mergeCell ref="C74:C84"/>
-    <mergeCell ref="D74:D84"/>
-    <mergeCell ref="A41:A49"/>
-    <mergeCell ref="B41:B49"/>
-    <mergeCell ref="C41:C49"/>
-    <mergeCell ref="D41:D49"/>
-    <mergeCell ref="A50:A60"/>
-    <mergeCell ref="B50:B60"/>
-    <mergeCell ref="C50:C60"/>
-    <mergeCell ref="D50:D60"/>
-    <mergeCell ref="A23:A32"/>
-    <mergeCell ref="B23:B32"/>
-    <mergeCell ref="C23:C32"/>
-    <mergeCell ref="D23:D32"/>
-    <mergeCell ref="A33:A40"/>
-    <mergeCell ref="B33:B40"/>
-    <mergeCell ref="C33:C40"/>
-    <mergeCell ref="D33:D40"/>
-    <mergeCell ref="A1:A10"/>
-    <mergeCell ref="B1:B10"/>
-    <mergeCell ref="C1:C10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A12:A22"/>
-    <mergeCell ref="B12:B22"/>
-    <mergeCell ref="C12:C22"/>
-    <mergeCell ref="D12:D22"/>
-    <mergeCell ref="A161:A167"/>
-    <mergeCell ref="B161:B167"/>
-    <mergeCell ref="C161:C167"/>
-    <mergeCell ref="D161:D167"/>
-    <mergeCell ref="A168:A174"/>
-    <mergeCell ref="B168:B174"/>
-    <mergeCell ref="C168:C174"/>
-    <mergeCell ref="D168:D174"/>
+    <mergeCell ref="A162:A168"/>
+    <mergeCell ref="B162:B168"/>
+    <mergeCell ref="C162:C168"/>
+    <mergeCell ref="D162:D168"/>
+    <mergeCell ref="A169:A175"/>
+    <mergeCell ref="B169:B175"/>
+    <mergeCell ref="C169:C175"/>
+    <mergeCell ref="D169:D175"/>
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="B2:B11"/>
+    <mergeCell ref="C2:C11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="D13:D23"/>
+    <mergeCell ref="A24:A33"/>
+    <mergeCell ref="B24:B33"/>
+    <mergeCell ref="C24:C33"/>
+    <mergeCell ref="D24:D33"/>
+    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="B34:B41"/>
+    <mergeCell ref="C34:C41"/>
+    <mergeCell ref="D34:D41"/>
+    <mergeCell ref="A42:A50"/>
+    <mergeCell ref="B42:B50"/>
+    <mergeCell ref="C42:C50"/>
+    <mergeCell ref="D42:D50"/>
+    <mergeCell ref="A51:A61"/>
+    <mergeCell ref="B51:B61"/>
+    <mergeCell ref="C51:C61"/>
+    <mergeCell ref="D51:D61"/>
+    <mergeCell ref="A62:A74"/>
+    <mergeCell ref="B62:B74"/>
+    <mergeCell ref="C62:C74"/>
+    <mergeCell ref="D62:D74"/>
+    <mergeCell ref="A75:A85"/>
+    <mergeCell ref="B75:B85"/>
+    <mergeCell ref="C75:C85"/>
+    <mergeCell ref="D75:D85"/>
+    <mergeCell ref="A86:A92"/>
+    <mergeCell ref="B86:B92"/>
+    <mergeCell ref="C86:C92"/>
+    <mergeCell ref="D86:D92"/>
+    <mergeCell ref="A93:A102"/>
+    <mergeCell ref="B93:B99"/>
+    <mergeCell ref="C93:C102"/>
+    <mergeCell ref="D93:D102"/>
+    <mergeCell ref="B100:B102"/>
+    <mergeCell ref="A103:A113"/>
+    <mergeCell ref="B103:B113"/>
+    <mergeCell ref="C103:C113"/>
+    <mergeCell ref="D103:D113"/>
+    <mergeCell ref="A114:A122"/>
+    <mergeCell ref="B114:B122"/>
+    <mergeCell ref="C114:C122"/>
+    <mergeCell ref="D114:D122"/>
+    <mergeCell ref="A123:A130"/>
+    <mergeCell ref="B123:B130"/>
+    <mergeCell ref="C123:C130"/>
+    <mergeCell ref="D123:D130"/>
+    <mergeCell ref="A131:A138"/>
+    <mergeCell ref="B131:B138"/>
+    <mergeCell ref="C131:C138"/>
+    <mergeCell ref="D131:D138"/>
+    <mergeCell ref="A155:A161"/>
+    <mergeCell ref="B155:B161"/>
+    <mergeCell ref="C155:C161"/>
+    <mergeCell ref="D155:D161"/>
+    <mergeCell ref="A139:A147"/>
+    <mergeCell ref="B139:B147"/>
+    <mergeCell ref="C139:C147"/>
+    <mergeCell ref="D139:D147"/>
+    <mergeCell ref="A148:A154"/>
+    <mergeCell ref="B148:B154"/>
+    <mergeCell ref="C148:C154"/>
+    <mergeCell ref="D148:D154"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A11" location="null!A38:A53" display="Section 3" xr:uid="{376511B3-A6BC-1F4C-A159-F713DB0BBEA3}"/>
+    <hyperlink ref="A12" location="null!A38:A53" display="Section 3" xr:uid="{376511B3-A6BC-1F4C-A159-F713DB0BBEA3}"/>
+    <hyperlink ref="A1" location="null!A1" display="Test Case ID" xr:uid="{4CE43408-3BC8-4AA0-9491-104999142F2E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>